<commit_message>
Fixed wrong coluumns names
</commit_message>
<xml_diff>
--- a/notebooks/ARIMA/predictions_ afr.xlsx
+++ b/notebooks/ARIMA/predictions_ afr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e012139a24c98f6/Рабочий стол/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sber\notebooks\ARIMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_304D1D541156BE0F62355476585DCE3A87479B7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8517B79-C1CD-4362-BCFF-240536A86A55}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB76B5E-A2DC-4A65-8C9A-322438B9828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,6 @@
     <t>Регион</t>
   </si>
   <si>
-    <t>Прогноз_СКР_2024</t>
-  </si>
-  <si>
-    <t>Факт_СКР_2024</t>
-  </si>
-  <si>
     <t>Абсолютная_ошибка</t>
   </si>
   <si>
@@ -293,6 +287,12 @@
   </si>
   <si>
     <t>г.Севастополь</t>
+  </si>
+  <si>
+    <t>predictions</t>
+  </si>
+  <si>
+    <t>СКР</t>
   </si>
 </sst>
 </file>
@@ -359,6 +359,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -375,10 +443,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="202020"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -658,40 +726,40 @@
   <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>1.2767999999999999</v>
@@ -709,9 +777,9 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.5387</v>
@@ -729,9 +797,9 @@
         <v>0.1017</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1.4410000000000001</v>
@@ -749,9 +817,9 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1.635</v>
@@ -769,9 +837,9 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1.123</v>
@@ -789,9 +857,9 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1.19</v>
@@ -809,9 +877,9 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1.147</v>
@@ -829,9 +897,9 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1.119</v>
@@ -849,9 +917,9 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1.391</v>
@@ -869,9 +937,9 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1.222</v>
@@ -889,9 +957,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1.5589999999999999</v>
@@ -909,9 +977,9 @@
         <v>0.216</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1.4939</v>
@@ -929,9 +997,9 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1.3460000000000001</v>
@@ -949,9 +1017,9 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1.65</v>
@@ -969,9 +1037,9 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1.526</v>
@@ -989,9 +1057,9 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1.1830000000000001</v>
@@ -1009,9 +1077,9 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>1.339</v>
@@ -1029,9 +1097,9 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1.6652</v>
@@ -1049,9 +1117,9 @@
         <v>7.7200000000000005E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1.34</v>
@@ -1069,9 +1137,9 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>1.1863999999999999</v>
@@ -1089,9 +1157,9 @@
         <v>2.3400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>1.4730000000000001</v>
@@ -1109,9 +1177,9 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1.552</v>
@@ -1129,9 +1197,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1.532</v>
@@ -1149,9 +1217,9 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1.4359999999999999</v>
@@ -1169,9 +1237,9 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>1.6419999999999999</v>
@@ -1189,9 +1257,9 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>1.262</v>
@@ -1209,9 +1277,9 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>0.88460000000000005</v>
@@ -1229,9 +1297,9 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1.2330000000000001</v>
@@ -1249,9 +1317,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>1.34</v>
@@ -1269,9 +1337,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>1.3520000000000001</v>
@@ -1289,9 +1357,9 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>1.4510000000000001</v>
@@ -1309,9 +1377,9 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>1.913</v>
@@ -1329,9 +1397,9 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>1.3089999999999999</v>
@@ -1349,9 +1417,9 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>1.2305999999999999</v>
@@ -1369,9 +1437,9 @@
         <v>2.06E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>1.492</v>
@@ -1389,9 +1457,9 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>1.4950000000000001</v>
@@ -1409,9 +1477,9 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>1.502</v>
@@ -1429,9 +1497,9 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>1.171</v>
@@ -1449,9 +1517,9 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>1.198</v>
@@ -1469,9 +1537,9 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>1.5269999999999999</v>
@@ -1489,9 +1557,9 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>1.444</v>
@@ -1509,9 +1577,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>1.3049999999999999</v>
@@ -1529,9 +1597,9 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>1.3460000000000001</v>
@@ -1549,9 +1617,9 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>1.9524999999999999</v>
@@ -1569,9 +1637,9 @@
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>1.3431</v>
@@ -1589,9 +1657,9 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>1.597</v>
@@ -1609,9 +1677,9 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>1.7450000000000001</v>
@@ -1629,9 +1697,9 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>1.8537999999999999</v>
@@ -1649,9 +1717,9 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>1.4430000000000001</v>
@@ -1669,9 +1737,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>1.534</v>
@@ -1689,9 +1757,9 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>1.6122000000000001</v>
@@ -1709,9 +1777,9 @@
         <v>8.4199999999999997E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>1.419</v>
@@ -1729,9 +1797,9 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>1.381</v>
@@ -1749,9 +1817,9 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>1.0469999999999999</v>
@@ -1769,9 +1837,9 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>1.5741000000000001</v>
@@ -1789,9 +1857,9 @@
         <v>1.3899999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>1.52</v>
@@ -1809,9 +1877,9 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>1.454</v>
@@ -1829,9 +1897,9 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>2.4420000000000002</v>
@@ -1849,9 +1917,9 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>1.482</v>
@@ -1869,9 +1937,9 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>1.272</v>
@@ -1889,9 +1957,9 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>1.1040000000000001</v>
@@ -1909,9 +1977,9 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>1.33</v>
@@ -1929,9 +1997,9 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>1.103</v>
@@ -1949,9 +2017,9 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>1.736</v>
@@ -1969,9 +2037,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>1.5509999999999999</v>
@@ -1989,9 +2057,9 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>1.0023</v>
@@ -2009,9 +2077,9 @@
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>1.2969999999999999</v>
@@ -2029,9 +2097,9 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>1.2070000000000001</v>
@@ -2049,9 +2117,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>1.2682</v>
@@ -2069,9 +2137,9 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>1.1506000000000001</v>
@@ -2089,9 +2157,9 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>1.2505999999999999</v>
@@ -2109,9 +2177,9 @@
         <v>0.1226</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>1.7098</v>
@@ -2129,9 +2197,9 @@
         <v>2.92E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>1.399</v>
@@ -2149,9 +2217,9 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>1.34</v>
@@ -2169,9 +2237,9 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>1.4645999999999999</v>
@@ -2189,9 +2257,9 @@
         <v>2.76E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>1.6701999999999999</v>
@@ -2209,9 +2277,9 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>1.4710000000000001</v>
@@ -2229,9 +2297,9 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>2.6899000000000002</v>
@@ -2249,9 +2317,9 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>1.4019999999999999</v>
@@ -2269,9 +2337,9 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>1.68</v>
@@ -2289,9 +2357,9 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>1.946</v>
@@ -2309,9 +2377,9 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>1.3160000000000001</v>
@@ -2329,9 +2397,9 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>1.3693</v>
@@ -2349,9 +2417,9 @@
         <v>9.1700000000000004E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>1.2569999999999999</v>
@@ -2369,9 +2437,9 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>0.95040000000000002</v>

</xml_diff>